<commit_message>
changes in the patient page
</commit_message>
<xml_diff>
--- a/client/src/data/patients/PA001.xlsx
+++ b/client/src/data/patients/PA001.xlsx
@@ -58,6 +58,12 @@
     <t>Observation</t>
   </si>
   <si>
+    <t>Protocole</t>
+  </si>
+  <si>
+    <t>P94C001FR</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
@@ -74,12 +80,6 @@
   </si>
   <si>
     <t>France</t>
-  </si>
-  <si>
-    <t>Protocole</t>
-  </si>
-  <si>
-    <t>P94C001FR</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1634,7 @@
       <c r="A10" t="s" s="26">
         <v>15</v>
       </c>
-      <c r="B10" t="s" s="15">
+      <c r="B10" t="s" s="20">
         <v>16</v>
       </c>
       <c r="C10" s="19"/>
@@ -1649,7 +1649,7 @@
       <c r="A11" t="s" s="26">
         <v>17</v>
       </c>
-      <c r="B11" t="s" s="20">
+      <c r="B11" t="s" s="15">
         <v>18</v>
       </c>
       <c r="C11" s="19"/>
@@ -1664,7 +1664,7 @@
       <c r="A12" t="s" s="26">
         <v>19</v>
       </c>
-      <c r="B12" t="s" s="15">
+      <c r="B12" t="s" s="20">
         <v>20</v>
       </c>
       <c r="C12" s="19"/>
@@ -1679,7 +1679,7 @@
       <c r="A13" t="s" s="26">
         <v>21</v>
       </c>
-      <c r="B13" t="s" s="20">
+      <c r="B13" t="s" s="15">
         <v>22</v>
       </c>
       <c r="C13" s="19"/>

</xml_diff>

<commit_message>
revoke consent page implemented
</commit_message>
<xml_diff>
--- a/client/src/data/patients/PA001.xlsx
+++ b/client/src/data/patients/PA001.xlsx
@@ -55,13 +55,13 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Observation</t>
+    <t>Trial</t>
   </si>
   <si>
     <t>Protocole</t>
   </si>
   <si>
-    <t>P94C001FR</t>
+    <t>P94A001FR</t>
   </si>
   <si>
     <t>ID</t>
@@ -277,7 +277,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -329,9 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -344,9 +341,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -354,6 +348,9 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1508,13 +1505,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="12">
-        <v>44332.650671296295</v>
+        <v>44333.039386574077</v>
       </c>
       <c r="E3" s="12">
-        <v>44332.653379629628</v>
+        <v>44333.253090277780</v>
       </c>
       <c r="F3" s="12">
-        <v>44332.655648148146</v>
+        <v>44333.253090277780</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="13"/>
@@ -1529,34 +1526,34 @@
       <c r="D4" s="16">
         <v>30</v>
       </c>
-      <c r="E4" s="17">
-        <v>30</v>
-      </c>
-      <c r="F4" s="17">
-        <v>30</v>
-      </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="E4" s="16">
+        <v>32</v>
+      </c>
+      <c r="F4" s="16">
+        <v>35</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" ht="22.2" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" t="s" s="20">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" t="s" s="19">
         <v>10</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>1.4</v>
       </c>
-      <c r="E5" s="22">
-        <v>1.6</v>
-      </c>
-      <c r="F5" s="22">
-        <v>1.5</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
+      <c r="E5" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1.1</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" ht="22.2" customHeight="1">
       <c r="A6" s="14"/>
@@ -1564,37 +1561,37 @@
       <c r="C6" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="22">
         <v>0.2</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="22">
         <v>0.1</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="22">
         <v>0.4</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" ht="22.2" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" t="s" s="20">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" t="s" s="19">
         <v>12</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="23">
         <v>0</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>0</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="23">
         <v>0</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" ht="22.2" customHeight="1">
       <c r="A8" s="14"/>
@@ -1602,93 +1599,93 @@
       <c r="C8" t="s" s="15">
         <v>13</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="24">
         <v>27</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="24">
         <v>27</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="24">
         <v>27</v>
       </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" ht="22.2" customHeight="1">
-      <c r="A9" t="s" s="26">
+      <c r="A9" t="s" s="25">
         <v>14</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>3</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" ht="22.2" customHeight="1">
-      <c r="A10" t="s" s="26">
+      <c r="A10" t="s" s="25">
         <v>15</v>
       </c>
-      <c r="B10" t="s" s="20">
+      <c r="B10" t="s" s="19">
         <v>16</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" ht="22.2" customHeight="1">
-      <c r="A11" t="s" s="26">
+      <c r="A11" t="s" s="25">
         <v>17</v>
       </c>
       <c r="B11" t="s" s="15">
         <v>18</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" ht="22.2" customHeight="1">
-      <c r="A12" t="s" s="26">
+      <c r="A12" t="s" s="25">
         <v>19</v>
       </c>
-      <c r="B12" t="s" s="20">
+      <c r="B12" t="s" s="19">
         <v>20</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" ht="22.2" customHeight="1">
-      <c r="A13" t="s" s="26">
+      <c r="A13" t="s" s="25">
         <v>21</v>
       </c>
       <c r="B13" t="s" s="15">
         <v>22</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
add alert to the smart contract
</commit_message>
<xml_diff>
--- a/client/src/data/patients/PA001.xlsx
+++ b/client/src/data/patients/PA001.xlsx
@@ -1505,14 +1505,12 @@
         <v>8</v>
       </c>
       <c r="D3" s="12">
-        <v>44333.039386574077</v>
+        <v>44334.963530092595</v>
       </c>
       <c r="E3" s="12">
-        <v>44333.253090277780</v>
-      </c>
-      <c r="F3" s="12">
-        <v>44333.253090277780</v>
-      </c>
+        <v>44334.963530092595</v>
+      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
@@ -1527,11 +1525,9 @@
         <v>30</v>
       </c>
       <c r="E4" s="16">
-        <v>32</v>
-      </c>
-      <c r="F4" s="16">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F4" s="14"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
@@ -1546,11 +1542,9 @@
         <v>1.4</v>
       </c>
       <c r="E5" s="20">
-        <v>1.2</v>
-      </c>
-      <c r="F5" s="20">
-        <v>1.1</v>
-      </c>
+        <v>1.4</v>
+      </c>
+      <c r="F5" s="18"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
@@ -1565,11 +1559,9 @@
         <v>0.2</v>
       </c>
       <c r="E6" s="22">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="22">
-        <v>0.4</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="22"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -1584,11 +1576,9 @@
         <v>0</v>
       </c>
       <c r="E7" s="23">
-        <v>0</v>
-      </c>
-      <c r="F7" s="23">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
@@ -1605,9 +1595,7 @@
       <c r="E8" s="24">
         <v>27</v>
       </c>
-      <c r="F8" s="24">
-        <v>27</v>
-      </c>
+      <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
@@ -1617,7 +1605,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>

</xml_diff>

<commit_message>
not user page changes
</commit_message>
<xml_diff>
--- a/client/src/data/patients/PA001.xlsx
+++ b/client/src/data/patients/PA001.xlsx
@@ -1505,12 +1505,14 @@
         <v>8</v>
       </c>
       <c r="D3" s="12">
-        <v>44334.963530092595</v>
+        <v>44336.358506944445</v>
       </c>
       <c r="E3" s="12">
-        <v>44334.963530092595</v>
-      </c>
-      <c r="F3" s="12"/>
+        <v>44336.361273148148</v>
+      </c>
+      <c r="F3" s="12">
+        <v>44336.363518518519</v>
+      </c>
       <c r="G3" s="12"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
@@ -1525,9 +1527,11 @@
         <v>30</v>
       </c>
       <c r="E4" s="16">
-        <v>30</v>
-      </c>
-      <c r="F4" s="14"/>
+        <v>32</v>
+      </c>
+      <c r="F4" s="16">
+        <v>31</v>
+      </c>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
@@ -1542,9 +1546,11 @@
         <v>1.4</v>
       </c>
       <c r="E5" s="20">
-        <v>1.4</v>
-      </c>
-      <c r="F5" s="18"/>
+        <v>1.2</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1.1</v>
+      </c>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
@@ -1559,9 +1565,11 @@
         <v>0.2</v>
       </c>
       <c r="E6" s="22">
-        <v>0.2</v>
-      </c>
-      <c r="F6" s="22"/>
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0.9</v>
+      </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -1576,9 +1584,11 @@
         <v>0</v>
       </c>
       <c r="E7" s="23">
+        <v>0</v>
+      </c>
+      <c r="F7" s="23">
         <v>1</v>
       </c>
-      <c r="F7" s="23"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
@@ -1595,7 +1605,9 @@
       <c r="E8" s="24">
         <v>27</v>
       </c>
-      <c r="F8" s="17"/>
+      <c r="F8" s="24">
+        <v>27</v>
+      </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
@@ -1605,7 +1617,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>

</xml_diff>